<commit_message>
add arp and op network
</commit_message>
<xml_diff>
--- a/app/templates/Bulk Payout Template.xlsx
+++ b/app/templates/Bulk Payout Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\project\EPUERP\code\desktop-agent\desktop-agent\app\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\project\EPUERP\code\BlockAtmGuard-github\blockatm-guard\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338BE833-C556-4047-AB9A-6DE239A8E2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B3131D-2500-463B-96D7-093E7E85A3B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2810,10 +2810,13 @@
       <formula>"dd-mm-yyyy h:mm "</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H3:H1001" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"DAI,USDT,USDC,TUSD,BUSD,FRAX,USDP,PAXG,GUSD"</formula1>
       <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 E3:E1048576" xr:uid="{20E5E44F-F017-464E-89E4-79097F874C7E}">
+      <formula1>"Ethereum Mainnet,Ethereum Goerli,TRON Shasta Testnet,TRON Mainnet,Arbitrum One Mainnet,Arbitrum Sepolia Testnet,Optimism Mainnet,Optimism Sepolia Testnet"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>